<commit_message>
Internalizando bibliotecas e imprimindo tabela de transicoes
</commit_message>
<xml_diff>
--- a/config/input.xlsx
+++ b/config/input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10120" windowWidth="24700" windowHeight="5440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="15620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PalavrasReservadas" sheetId="1" r:id="rId1"/>
@@ -792,7 +792,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -806,7 +805,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1042,7 +1041,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:I8" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
modificando analisador lexico para entrega 2
</commit_message>
<xml_diff>
--- a/config/input.xlsx
+++ b/config/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24660" windowHeight="15620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PalavrasReservadas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>if</t>
   </si>
@@ -141,6 +141,33 @@
   </si>
   <si>
     <t>1,6</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -594,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -672,6 +699,54 @@
       </c>
       <c r="B9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -686,10 +761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -788,6 +863,30 @@
       </c>
       <c r="B12" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ainda corrigindo essa ...
</commit_message>
<xml_diff>
--- a/config/input.xlsx
+++ b/config/input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15040" yWindow="0" windowWidth="12940" windowHeight="15620" tabRatio="884" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24640" windowHeight="15620" tabRatio="884" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PalavrasReservadas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="5.Indiretas" sheetId="18" r:id="rId18"/>
     <sheet name="6.Indiretas" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="98">
   <si>
     <t>if</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>2,6</t>
   </si>
 </sst>
 </file>
@@ -1589,7 +1592,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2997,7 +2999,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3011,7 +3012,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M8"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3105,7 +3106,7 @@
       </c>
       <c r="M2" s="22" t="str">
         <f>TEXT(Automatos!M72, "##")</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -3183,19 +3184,19 @@
       </c>
       <c r="F4" s="22" t="str">
         <f>TEXT(Automatos!F74, "##")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G4" s="22" t="str">
         <f>TEXT(Automatos!G74, "##")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H4" s="22" t="str">
         <f>TEXT(Automatos!H74, "##")</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="I4" s="22" t="str">
         <f>TEXT(Automatos!I74, "##")</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="J4" s="22" t="str">
         <f>TEXT(Automatos!J74, "##")</f>
@@ -3203,11 +3204,11 @@
       </c>
       <c r="K4" s="22" t="str">
         <f>TEXT(Automatos!K74, "##")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L4" s="22" t="str">
         <f>TEXT(Automatos!L74, "##")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M4" s="22" t="str">
         <f>TEXT(Automatos!M74, "##")</f>
@@ -3236,19 +3237,19 @@
       </c>
       <c r="F5" s="22" t="str">
         <f>TEXT(Automatos!F75, "##")</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="G5" s="22" t="str">
         <f>TEXT(Automatos!G75, "##")</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="H5" s="22" t="str">
         <f>TEXT(Automatos!H75, "##")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="I5" s="22" t="str">
         <f>TEXT(Automatos!I75, "##")</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="J5" s="22" t="str">
         <f>TEXT(Automatos!J75, "##")</f>
@@ -3256,11 +3257,11 @@
       </c>
       <c r="K5" s="22" t="str">
         <f>TEXT(Automatos!K75, "##")</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="L5" s="22" t="str">
         <f>TEXT(Automatos!L75, "##")</f>
-        <v>6</v>
+        <v/>
       </c>
       <c r="M5" s="22" t="str">
         <f>TEXT(Automatos!M75, "##")</f>
@@ -3289,7 +3290,7 @@
       </c>
       <c r="F6" s="22" t="str">
         <f>TEXT(Automatos!F76, "##")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G6" s="22" t="str">
         <f>TEXT(Automatos!G76, "##")</f>
@@ -3395,7 +3396,7 @@
       </c>
       <c r="F8" s="22" t="str">
         <f>TEXT(Automatos!F78, "##")</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="G8" s="22" t="str">
         <f>TEXT(Automatos!G78, "##")</f>
@@ -3415,11 +3416,11 @@
       </c>
       <c r="K8" s="22" t="str">
         <f>TEXT(Automatos!K78, "##")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="L8" s="22" t="str">
         <f>TEXT(Automatos!L78, "##")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="M8" s="22" t="str">
         <f>TEXT(Automatos!M78, "##")</f>
@@ -3428,7 +3429,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3662,7 +3662,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3976,7 +3975,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4000,7 +3999,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -4011,29 +4010,29 @@
         <v>6</v>
       </c>
       <c r="C3" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>6</v>
       </c>
       <c r="C4" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
         <v>6</v>
       </c>
       <c r="C5" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4044,7 +4043,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4503,8 +4502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5909,9 +5908,6 @@
       <c r="J72" s="8">
         <v>1</v>
       </c>
-      <c r="M72" s="8">
-        <v>2</v>
-      </c>
       <c r="S72" s="16"/>
       <c r="T72" s="16"/>
       <c r="U72" s="16"/>
@@ -5931,11 +5927,23 @@
       <c r="A74" s="9">
         <v>2</v>
       </c>
+      <c r="F74" s="8">
+        <v>3</v>
+      </c>
+      <c r="G74" s="8">
+        <v>3</v>
+      </c>
+      <c r="H74" s="8">
+        <v>4</v>
+      </c>
+      <c r="I74" s="8">
+        <v>4</v>
+      </c>
       <c r="K74" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L74" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S74" s="16"/>
       <c r="T74" s="16"/>
@@ -5945,24 +5953,6 @@
       <c r="A75" s="9">
         <v>3</v>
       </c>
-      <c r="F75" s="8">
-        <v>4</v>
-      </c>
-      <c r="G75" s="8">
-        <v>4</v>
-      </c>
-      <c r="H75" s="8">
-        <v>5</v>
-      </c>
-      <c r="I75" s="8">
-        <v>5</v>
-      </c>
-      <c r="K75" s="8">
-        <v>6</v>
-      </c>
-      <c r="L75" s="8">
-        <v>6</v>
-      </c>
       <c r="S75" s="16"/>
       <c r="T75" s="16"/>
       <c r="U75" s="16"/>
@@ -5971,6 +5961,9 @@
       <c r="A76" s="9">
         <v>4</v>
       </c>
+      <c r="F76" s="8">
+        <v>3</v>
+      </c>
       <c r="S76" s="16"/>
       <c r="T76" s="16"/>
       <c r="U76" s="16"/>
@@ -5987,8 +5980,11 @@
       <c r="A78" s="9">
         <v>6</v>
       </c>
-      <c r="F78" s="8">
-        <v>4</v>
+      <c r="K78" s="8">
+        <v>5</v>
+      </c>
+      <c r="L78" s="8">
+        <v>5</v>
       </c>
       <c r="S78" s="16"/>
       <c r="T78" s="16"/>
@@ -6136,7 +6132,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6663,7 +6658,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7148,7 +7142,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7220,7 +7214,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -7236,7 +7230,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8175,7 +8168,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8540,7 +8532,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Alteracao no programa fonte. Espacamento de tokens
</commit_message>
<xml_diff>
--- a/config/input.xlsx
+++ b/config/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="0" windowWidth="18580" windowHeight="15620" tabRatio="884" firstSheet="3" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24640" windowHeight="15620" tabRatio="884" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PalavrasReservadas" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="99">
   <si>
     <t>if</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>10,21</t>
+  </si>
+  <si>
+    <t>Numero</t>
   </si>
 </sst>
 </file>
@@ -1656,7 +1659,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3064,7 +3066,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3495,7 +3496,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3508,7 +3508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3729,7 +3729,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6772,8 +6771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6802,7 +6801,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="B3" s="12">
         <v>257</v>
@@ -8398,7 +8397,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8763,7 +8761,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>